<commit_message>
adding modified class files
</commit_message>
<xml_diff>
--- a/dev/ZYCUS/src/main/TestCases/Zycus-Assignment.xlsx
+++ b/dev/ZYCUS/src/main/TestCases/Zycus-Assignment.xlsx
@@ -247,15 +247,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,7 +593,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,25 +608,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -644,32 +640,32 @@
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -679,20 +675,20 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -702,20 +698,20 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -725,20 +721,20 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -757,10 +753,11 @@
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -768,17 +765,18 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G8" s="1" t="s">

</xml_diff>